<commit_message>
sanunits for Biogenic Refinery added
</commit_message>
<xml_diff>
--- a/qsdsan/data/_impact_item.xlsx
+++ b/qsdsan/data/_impact_item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/qs_yl/qsdsan/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewisrowles/Dropbox/My Mac (Lewiss-MBP.lan1)/Documents/UIUC/Gates/QSDsan/QSD_adding_biogenic_refinery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2A4D037B-7307-C842-B5BB-8B02115339E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD125218-1BDF-DD41-9654-4BB0F70EBE42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="2260" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="27240" windowHeight="16080" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -116,6 +116,45 @@
   </si>
   <si>
     <t>Trucking</t>
+  </si>
+  <si>
+    <t>ea</t>
+  </si>
+  <si>
+    <t>ElectricMotor</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>CatalyticConverter</t>
+  </si>
+  <si>
+    <t>OilHeatExchanger</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>HydronicHeatExchanger</t>
+  </si>
+  <si>
+    <t>ElectricConnectors</t>
+  </si>
+  <si>
+    <t>ElectricCables</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>PVC</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>Polyacrylamide</t>
   </si>
 </sst>
 </file>
@@ -506,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,6 +661,80 @@
         <v>24</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -629,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28627DAA-889C-6942-A3B5-3C8A993554C1}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,6 +1068,259 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3">
+        <v>9.9703471209999996</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8.9733124089</v>
+      </c>
+      <c r="E14" s="3">
+        <v>10.967381833100001</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8.8474600330000008</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7.9627140297000008</v>
+      </c>
+      <c r="E15" s="3">
+        <v>9.7322060363000009</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13.937562</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12.543805799999999</v>
+      </c>
+      <c r="E16" s="3">
+        <v>15.3313182</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3">
+        <v>114014.66383541599</v>
+      </c>
+      <c r="D17" s="3">
+        <v>102613.1974518744</v>
+      </c>
+      <c r="E17" s="3">
+        <v>125416.13021895761</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3">
+        <v>8.5937041260028693</v>
+      </c>
+      <c r="D18" s="3">
+        <v>7.7343337134025827</v>
+      </c>
+      <c r="E18" s="3">
+        <v>9.4530745386031576</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3">
+        <v>324.96867299992499</v>
+      </c>
+      <c r="D19" s="3">
+        <v>292.47180569993247</v>
+      </c>
+      <c r="E19" s="3">
+        <v>357.46554029991751</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="3">
+        <v>8.8474600327818393</v>
+      </c>
+      <c r="D20" s="3">
+        <v>7.9627140295036556</v>
+      </c>
+      <c r="E20" s="3">
+        <v>9.732206036060024</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4.3790218750000003</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3.9411196875000005</v>
+      </c>
+      <c r="E21" s="3">
+        <v>4.8169240625000009</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2.797495751</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2.5177461759000002</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3.0772453261000003</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G12">
     <sortCondition ref="A3:A12"/>

</xml_diff>